<commit_message>
Added comparer for barcodes. Under ScanPage class
</commit_message>
<xml_diff>
--- a/barcodes.xlsx
+++ b/barcodes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spenc\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spenc\Source\Repos\jmerolla\470-Box-Picking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D6524E-52CE-49AE-AA41-3DFC01D72770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C9008D-1FF2-4F16-9225-2CC35C1C48F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37880" yWindow="650" windowWidth="28800" windowHeight="15540" xr2:uid="{B968A885-ED39-48AB-A812-D27A967B124A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B968A885-ED39-48AB-A812-D27A967B124A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Products</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>Barcode</t>
+  </si>
+  <si>
+    <t>Acrylic2.0mil FOIL</t>
+  </si>
+  <si>
+    <t>5561600741</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4"-50yards</t>
   </si>
 </sst>
 </file>
@@ -419,20 +431,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC3B7B2-192D-4A8E-9238-7A1C02A21A44}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,8 +455,11 @@
       <c r="C1" t="s">
         <v>8</v>
       </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -455,7 +471,7 @@
         <v>*121457814952*</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -463,11 +479,11 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="str">
-        <f t="shared" ref="C3:C4" si="0">"*"&amp;B3&amp;"*"</f>
+        <f t="shared" ref="C3:C5" si="0">"*"&amp;B3&amp;"*"</f>
         <v>*213212333347*</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -477,6 +493,21 @@
       <c r="C4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>*247586943784*</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>*5561600741*</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>